<commit_message>
grade sheet condition resolved
</commit_message>
<xml_diff>
--- a/public/assets/files/Grade-Sheet-Format.xlsx
+++ b/public/assets/files/Grade-Sheet-Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755ebb071ff8026e/__eGradeNav__ - Final/client/public/assets/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755ebb071ff8026e/__eGradeNav__ - Final - backup 1 - Copy/client/public/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{D3E580A8-84D3-4BDD-8362-31F3D60BB9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E37B861-50FC-45A3-892D-19C50EE4989F}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{D3E580A8-84D3-4BDD-8362-31F3D60BB9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4DB444D-34E8-4CF9-BFFC-86A412DA0D09}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,9 +545,82 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,18 +681,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,19 +688,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -650,56 +700,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,7 +1095,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27:N27"/>
+      <selection activeCell="I26" sqref="I26:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1154,30 +1154,30 @@
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="55" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="49" t="s">
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="51"/>
+      <c r="P7" s="79"/>
+      <c r="Q7" s="79"/>
+      <c r="R7" s="80"/>
     </row>
     <row r="8" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -1214,10 +1214,10 @@
       <c r="N8" s="13">
         <v>84</v>
       </c>
-      <c r="O8" s="52"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="54"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="83"/>
     </row>
     <row r="9" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
@@ -1256,10 +1256,10 @@
       <c r="N9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="52"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="54"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="83"/>
     </row>
     <row r="10" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
@@ -1299,10 +1299,10 @@
       <c r="N10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O10" s="52"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="54"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="83"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
@@ -1339,12 +1339,12 @@
       <c r="N11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="55" t="s">
+      <c r="O11" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="57"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="44"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -1385,9 +1385,9 @@
       <c r="O12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="70"/>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="72"/>
+      <c r="P12" s="90"/>
+      <c r="Q12" s="90"/>
+      <c r="R12" s="92"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1432,9 +1432,9 @@
       <c r="O13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="57"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="44"/>
     </row>
     <row r="14" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
@@ -1490,17 +1490,17 @@
       <c r="K15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="67" t="s">
+      <c r="L15" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="68"/>
-      <c r="N15" s="69"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="89"/>
       <c r="O15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="59"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="84"/>
     </row>
     <row r="16" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
@@ -1509,36 +1509,36 @@
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
-      <c r="J16" s="70" t="s">
+      <c r="J16" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="70"/>
-      <c r="L16" s="71" t="s">
+      <c r="K16" s="90"/>
+      <c r="L16" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="70"/>
-      <c r="N16" s="72"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="92"/>
       <c r="O16" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="59"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="84"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="42"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="71"/>
       <c r="O17" s="14"/>
       <c r="R17" s="8"/>
     </row>
@@ -1550,34 +1550,34 @@
         <v>11</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="44"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="60" t="s">
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="45"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="74"/>
       <c r="O19" s="14"/>
       <c r="Q19" s="24" t="s">
         <v>47</v>
@@ -1590,75 +1590,75 @@
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="61" t="s">
+      <c r="F20" s="75"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="63"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="87"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="79" t="s">
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="80"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="64" t="s">
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="34" t="s">
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="36"/>
+      <c r="Q21" s="64"/>
+      <c r="R21" s="65"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="55" t="s">
+      <c r="A22" s="53"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="56"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="55" t="s">
+      <c r="J22" s="43"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="M22" s="56"/>
-      <c r="N22" s="57"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="44"/>
       <c r="O22" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="39"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="68"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
@@ -1668,19 +1668,19 @@
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
       <c r="E23" s="30"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
       <c r="O23" s="31"/>
-      <c r="P23" s="85"/>
-      <c r="Q23" s="85"/>
-      <c r="R23" s="85"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="32">
@@ -1690,22 +1690,25 @@
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="73"/>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
-      <c r="O24" s="92" t="str" cm="1">
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="34" t="str" cm="1">
         <f t="array" ref="O24">IF(COUNT(I24:N24)=0,"",(SUM((I24:N24)/2)-0.01))</f>
         <v/>
       </c>
-      <c r="P24" s="85"/>
-      <c r="Q24" s="85"/>
-      <c r="R24" s="85"/>
+      <c r="P24" s="35" t="str">
+        <f>IF(OR(I24="ODRP", L24="ODRP"), "ODRP", IF(OR(I24="INC", L24="INC"), "INC", ""))</f>
+        <v/>
+      </c>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="26">
@@ -1716,65 +1719,83 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="85"/>
-      <c r="Q25" s="85"/>
-      <c r="R25" s="85"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="34" t="str" cm="1">
+        <f t="array" ref="O25">IF(COUNT(I25:N25)=0,"",(SUM((I25:N25)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P25" s="35" t="str">
+        <f t="shared" ref="P25:P29" si="5">IF(OR(I25="ODRP", L25="ODRP"), "ODRP", IF(OR(I25="INC", L25="INC"), "INC", ""))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="26">
-        <f t="shared" ref="A26:A27" si="5">A25+1</f>
+        <f t="shared" ref="A26:A27" si="6">A25+1</f>
         <v>3</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="30"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="85"/>
-      <c r="Q26" s="85"/>
-      <c r="R26" s="85"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="34" t="str" cm="1">
+        <f t="array" ref="O26">IF(COUNT(I26:N26)=0,"",(SUM((I26:N26)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P26" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="85"/>
-      <c r="Q27" s="85"/>
-      <c r="R27" s="85"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="34" t="str" cm="1">
+        <f t="array" ref="O27">IF(COUNT(I27:N27)=0,"",(SUM((I27:N27)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P27" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="26">
@@ -1785,19 +1806,25 @@
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="30"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73"/>
-      <c r="N28" s="73"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="85"/>
-      <c r="R28" s="85"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="34" t="str" cm="1">
+        <f t="array" ref="O28">IF(COUNT(I28:N28)=0,"",(SUM((I28:N28)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P28" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="26">
@@ -1808,111 +1835,129 @@
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="30"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="85"/>
-      <c r="Q29" s="85"/>
-      <c r="R29" s="85"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="34" t="str" cm="1">
+        <f t="array" ref="O29">IF(COUNT(I29:N29)=0,"",(SUM((I29:N29)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P29" s="35" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="26">
-        <f t="shared" ref="A30:A33" si="6">A29+1</f>
+        <f t="shared" ref="A30:A33" si="7">A29+1</f>
         <v>7</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="30"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="88"/>
-      <c r="N30" s="89"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="85"/>
-      <c r="Q30" s="85"/>
-      <c r="R30" s="85"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="34" t="str" cm="1">
+        <f t="array" ref="O30">IF(COUNT(I30:N30)=0,"",(SUM((I30:N30)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="30"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="89"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="85"/>
-      <c r="Q31" s="85"/>
-      <c r="R31" s="85"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="34" t="str" cm="1">
+        <f t="array" ref="O31">IF(COUNT(I31:N31)=0,"",(SUM((I31:N31)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="B32" s="31"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="85"/>
-      <c r="J32" s="85"/>
-      <c r="K32" s="85"/>
-      <c r="L32" s="85"/>
-      <c r="M32" s="85"/>
-      <c r="N32" s="85"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="85"/>
-      <c r="Q32" s="85"/>
-      <c r="R32" s="85"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="34" t="str" cm="1">
+        <f t="array" ref="O32">IF(COUNT(I32:N32)=0,"",(SUM((I32:N32)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="B33" s="31"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="30"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="85"/>
-      <c r="L33" s="85"/>
-      <c r="M33" s="85"/>
-      <c r="N33" s="85"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="85"/>
-      <c r="Q33" s="85"/>
-      <c r="R33" s="85"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="34" t="str" cm="1">
+        <f t="array" ref="O33">IF(COUNT(I33:N33)=0,"",(SUM((I33:N33)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
@@ -1922,19 +1967,22 @@
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="85"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="85"/>
-      <c r="M34" s="85"/>
-      <c r="N34" s="85"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="85"/>
-      <c r="Q34" s="85"/>
-      <c r="R34" s="85"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="34" t="str" cm="1">
+        <f t="array" ref="O34">IF(COUNT(I34:N34)=0,"",(SUM((I34:N34)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="26">
@@ -1944,19 +1992,22 @@
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="30"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="85"/>
-      <c r="M35" s="85"/>
-      <c r="N35" s="85"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="85"/>
-      <c r="Q35" s="85"/>
-      <c r="R35" s="85"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="34" t="str" cm="1">
+        <f t="array" ref="O35">IF(COUNT(I35:N35)=0,"",(SUM((I35:N35)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="26">
@@ -1967,203 +2018,230 @@
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
       <c r="E36" s="30"/>
-      <c r="F36" s="85"/>
-      <c r="G36" s="85"/>
-      <c r="H36" s="85"/>
-      <c r="I36" s="85"/>
-      <c r="J36" s="85"/>
-      <c r="K36" s="85"/>
-      <c r="L36" s="85"/>
-      <c r="M36" s="85"/>
-      <c r="N36" s="85"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="85"/>
-      <c r="Q36" s="85"/>
-      <c r="R36" s="85"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="34" t="str" cm="1">
+        <f t="array" ref="O36">IF(COUNT(I36:N36)=0,"",(SUM((I36:N36)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
-        <f t="shared" ref="A37:A44" si="7">A36+1</f>
+        <f t="shared" ref="A37:A44" si="8">A36+1</f>
         <v>3</v>
       </c>
       <c r="B37" s="31"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="30"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="85"/>
-      <c r="K37" s="85"/>
-      <c r="L37" s="85"/>
-      <c r="M37" s="85"/>
-      <c r="N37" s="85"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="85"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="85"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="34" t="str" cm="1">
+        <f t="array" ref="O37">IF(COUNT(I37:N37)=0,"",(SUM((I37:N37)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="B38" s="31"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="30"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="85"/>
-      <c r="M38" s="85"/>
-      <c r="N38" s="85"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="85"/>
-      <c r="Q38" s="85"/>
-      <c r="R38" s="85"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="34" t="str" cm="1">
+        <f t="array" ref="O38">IF(COUNT(I38:N38)=0,"",(SUM((I38:N38)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="30"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="85"/>
-      <c r="L39" s="85"/>
-      <c r="M39" s="85"/>
-      <c r="N39" s="85"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="85"/>
-      <c r="Q39" s="85"/>
-      <c r="R39" s="85"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="34" t="str" cm="1">
+        <f t="array" ref="O39">IF(COUNT(I39:N39)=0,"",(SUM((I39:N39)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="30"/>
-      <c r="F40" s="85"/>
-      <c r="G40" s="85"/>
-      <c r="H40" s="85"/>
-      <c r="I40" s="85"/>
-      <c r="J40" s="85"/>
-      <c r="K40" s="85"/>
-      <c r="L40" s="85"/>
-      <c r="M40" s="85"/>
-      <c r="N40" s="85"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="85"/>
-      <c r="Q40" s="85"/>
-      <c r="R40" s="85"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="34" t="str" cm="1">
+        <f t="array" ref="O40">IF(COUNT(I40:N40)=0,"",(SUM((I40:N40)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="B41" s="31"/>
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
       <c r="E41" s="30"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
-      <c r="H41" s="85"/>
-      <c r="I41" s="85"/>
-      <c r="J41" s="85"/>
-      <c r="K41" s="85"/>
-      <c r="L41" s="85"/>
-      <c r="M41" s="85"/>
-      <c r="N41" s="85"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="85"/>
-      <c r="Q41" s="85"/>
-      <c r="R41" s="85"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="34" t="str" cm="1">
+        <f t="array" ref="O41">IF(COUNT(I41:N41)=0,"",(SUM((I41:N41)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="B42" s="31"/>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="30"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="85"/>
-      <c r="K42" s="85"/>
-      <c r="L42" s="85"/>
-      <c r="M42" s="85"/>
-      <c r="N42" s="85"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="85"/>
-      <c r="Q42" s="85"/>
-      <c r="R42" s="85"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="34" t="str" cm="1">
+        <f t="array" ref="O42">IF(COUNT(I42:N42)=0,"",(SUM((I42:N42)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="85"/>
-      <c r="I43" s="85"/>
-      <c r="J43" s="85"/>
-      <c r="K43" s="85"/>
-      <c r="L43" s="85"/>
-      <c r="M43" s="85"/>
-      <c r="N43" s="85"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="85"/>
-      <c r="Q43" s="85"/>
-      <c r="R43" s="85"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="34" t="str" cm="1">
+        <f t="array" ref="O43">IF(COUNT(I43:N43)=0,"",(SUM((I43:N43)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="B44" s="33"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="85"/>
-      <c r="H44" s="85"/>
-      <c r="I44" s="85"/>
-      <c r="J44" s="85"/>
-      <c r="K44" s="85"/>
-      <c r="L44" s="85"/>
-      <c r="M44" s="85"/>
-      <c r="N44" s="85"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="85"/>
-      <c r="Q44" s="85"/>
-      <c r="R44" s="85"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="34" t="str" cm="1">
+        <f t="array" ref="O44">IF(COUNT(I44:N44)=0,"",(SUM((I44:N44)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="35"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="27"/>
@@ -2171,19 +2249,22 @@
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="30"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
-      <c r="M45" s="85"/>
-      <c r="N45" s="85"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="85"/>
-      <c r="Q45" s="85"/>
-      <c r="R45" s="85"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="34" t="str" cm="1">
+        <f t="array" ref="O45">IF(COUNT(I45:N45)=0,"",(SUM((I45:N45)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P45" s="35"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="35"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="27"/>
@@ -2191,19 +2272,22 @@
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
       <c r="E46" s="30"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="85"/>
-      <c r="J46" s="85"/>
-      <c r="K46" s="85"/>
-      <c r="L46" s="85"/>
-      <c r="M46" s="85"/>
-      <c r="N46" s="85"/>
-      <c r="O46" s="27"/>
-      <c r="P46" s="85"/>
-      <c r="Q46" s="85"/>
-      <c r="R46" s="85"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="34" t="str" cm="1">
+        <f t="array" ref="O46">IF(COUNT(I46:N46)=0,"",(SUM((I46:N46)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="35"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
@@ -2211,19 +2295,22 @@
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="30"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="85"/>
-      <c r="K47" s="85"/>
-      <c r="L47" s="85"/>
-      <c r="M47" s="85"/>
-      <c r="N47" s="85"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="85"/>
-      <c r="Q47" s="85"/>
-      <c r="R47" s="85"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
+      <c r="O47" s="34" t="str" cm="1">
+        <f t="array" ref="O47">IF(COUNT(I47:N47)=0,"",(SUM((I47:N47)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P47" s="35"/>
+      <c r="Q47" s="35"/>
+      <c r="R47" s="35"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="27"/>
@@ -2231,19 +2318,22 @@
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
       <c r="E48" s="30"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
-      <c r="K48" s="85"/>
-      <c r="L48" s="85"/>
-      <c r="M48" s="85"/>
-      <c r="N48" s="85"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="85"/>
-      <c r="Q48" s="85"/>
-      <c r="R48" s="85"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="34" t="str" cm="1">
+        <f t="array" ref="O48">IF(COUNT(I48:N48)=0,"",(SUM((I48:N48)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="35"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="27"/>
@@ -2251,19 +2341,22 @@
       <c r="C49" s="29"/>
       <c r="D49" s="29"/>
       <c r="E49" s="30"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="85"/>
-      <c r="M49" s="85"/>
-      <c r="N49" s="85"/>
-      <c r="O49" s="27"/>
-      <c r="P49" s="85"/>
-      <c r="Q49" s="85"/>
-      <c r="R49" s="85"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="34" t="str" cm="1">
+        <f t="array" ref="O49">IF(COUNT(I49:N49)=0,"",(SUM((I49:N49)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P49" s="35"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="35"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="27"/>
@@ -2271,19 +2364,22 @@
       <c r="C50" s="29"/>
       <c r="D50" s="29"/>
       <c r="E50" s="30"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="85"/>
-      <c r="K50" s="85"/>
-      <c r="L50" s="85"/>
-      <c r="M50" s="85"/>
-      <c r="N50" s="85"/>
-      <c r="O50" s="27"/>
-      <c r="P50" s="85"/>
-      <c r="Q50" s="85"/>
-      <c r="R50" s="85"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="34" t="str" cm="1">
+        <f t="array" ref="O50">IF(COUNT(I50:N50)=0,"",(SUM((I50:N50)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P50" s="35"/>
+      <c r="Q50" s="35"/>
+      <c r="R50" s="35"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="27"/>
@@ -2291,19 +2387,22 @@
       <c r="C51" s="29"/>
       <c r="D51" s="29"/>
       <c r="E51" s="30"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="85"/>
-      <c r="I51" s="85"/>
-      <c r="J51" s="85"/>
-      <c r="K51" s="85"/>
-      <c r="L51" s="85"/>
-      <c r="M51" s="85"/>
-      <c r="N51" s="85"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="85"/>
-      <c r="Q51" s="85"/>
-      <c r="R51" s="85"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="34" t="str" cm="1">
+        <f t="array" ref="O51">IF(COUNT(I51:N51)=0,"",(SUM((I51:N51)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
@@ -2311,19 +2410,22 @@
       <c r="C52" s="29"/>
       <c r="D52" s="29"/>
       <c r="E52" s="30"/>
-      <c r="F52" s="85"/>
-      <c r="G52" s="85"/>
-      <c r="H52" s="85"/>
-      <c r="I52" s="85"/>
-      <c r="J52" s="85"/>
-      <c r="K52" s="85"/>
-      <c r="L52" s="85"/>
-      <c r="M52" s="85"/>
-      <c r="N52" s="85"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="85"/>
-      <c r="Q52" s="85"/>
-      <c r="R52" s="85"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="34" t="str" cm="1">
+        <f t="array" ref="O52">IF(COUNT(I52:N52)=0,"",(SUM((I52:N52)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P52" s="35"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="35"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="27"/>
@@ -2331,19 +2433,22 @@
       <c r="C53" s="29"/>
       <c r="D53" s="29"/>
       <c r="E53" s="30"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="85"/>
-      <c r="I53" s="85"/>
-      <c r="J53" s="85"/>
-      <c r="K53" s="85"/>
-      <c r="L53" s="85"/>
-      <c r="M53" s="85"/>
-      <c r="N53" s="85"/>
-      <c r="O53" s="27"/>
-      <c r="P53" s="85"/>
-      <c r="Q53" s="85"/>
-      <c r="R53" s="85"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="34" t="str" cm="1">
+        <f t="array" ref="O53">IF(COUNT(I53:N53)=0,"",(SUM((I53:N53)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P53" s="35"/>
+      <c r="Q53" s="35"/>
+      <c r="R53" s="35"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="27"/>
@@ -2351,19 +2456,22 @@
       <c r="C54" s="29"/>
       <c r="D54" s="29"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="85"/>
-      <c r="M54" s="85"/>
-      <c r="N54" s="85"/>
-      <c r="O54" s="27"/>
-      <c r="P54" s="85"/>
-      <c r="Q54" s="85"/>
-      <c r="R54" s="85"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="34" t="str" cm="1">
+        <f t="array" ref="O54">IF(COUNT(I54:N54)=0,"",(SUM((I54:N54)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="35"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="27"/>
@@ -2371,217 +2479,290 @@
       <c r="C55" s="29"/>
       <c r="D55" s="29"/>
       <c r="E55" s="30"/>
-      <c r="F55" s="85"/>
-      <c r="G55" s="85"/>
-      <c r="H55" s="85"/>
-      <c r="I55" s="85"/>
-      <c r="J55" s="85"/>
-      <c r="K55" s="85"/>
-      <c r="L55" s="85"/>
-      <c r="M55" s="85"/>
-      <c r="N55" s="85"/>
-      <c r="O55" s="27"/>
-      <c r="P55" s="85"/>
-      <c r="Q55" s="85"/>
-      <c r="R55" s="85"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="34" t="str" cm="1">
+        <f t="array" ref="O55">IF(COUNT(I55:N55)=0,"",(SUM((I55:N55)/2)-0.01))</f>
+        <v/>
+      </c>
+      <c r="P55" s="35"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="35"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="55" t="s">
+      <c r="A56" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
-      <c r="J56" s="56"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
-      <c r="O56" s="56"/>
-      <c r="P56" s="56"/>
-      <c r="Q56" s="56"/>
-      <c r="R56" s="57"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="44"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
-      <c r="K57" s="68"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="58" t="s">
+      <c r="A58" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="58"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="68"/>
-      <c r="I58" s="68"/>
-      <c r="J58" s="68"/>
-      <c r="K58" s="68"/>
+      <c r="B58" s="39"/>
+      <c r="F58" s="36"/>
+      <c r="G58" s="36"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="36"/>
+      <c r="J58" s="36"/>
+      <c r="K58" s="36"/>
       <c r="N58" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P58" s="68"/>
-      <c r="Q58" s="68"/>
-      <c r="R58" s="68"/>
+      <c r="P58" s="36"/>
+      <c r="Q58" s="36"/>
+      <c r="R58" s="36"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="77"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="77"/>
-      <c r="F59" s="77"/>
-      <c r="G59" s="77"/>
-      <c r="H59" s="77"/>
-      <c r="I59" s="68"/>
-      <c r="J59" s="68"/>
-      <c r="K59" s="68"/>
-      <c r="L59" s="68"/>
-      <c r="M59" s="68"/>
-      <c r="N59" s="68"/>
-      <c r="O59" s="77"/>
-      <c r="P59" s="77"/>
-      <c r="Q59" s="77"/>
-      <c r="R59" s="77"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="36"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="36"/>
+      <c r="N59" s="36"/>
+      <c r="O59" s="40"/>
+      <c r="P59" s="40"/>
+      <c r="Q59" s="40"/>
+      <c r="R59" s="40"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="86" t="s">
+      <c r="B60" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="C60" s="86"/>
-      <c r="D60" s="86"/>
-      <c r="E60" s="86"/>
-      <c r="F60" s="86"/>
-      <c r="G60" s="86"/>
-      <c r="H60" s="86"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="91" t="s">
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="P60" s="91"/>
-      <c r="Q60" s="91"/>
-      <c r="R60" s="91"/>
+      <c r="P60" s="41"/>
+      <c r="Q60" s="41"/>
+      <c r="R60" s="41"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E63" s="58" t="s">
+      <c r="E63" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="68"/>
-      <c r="J63" s="68"/>
-      <c r="K63" s="68"/>
-      <c r="L63" s="68"/>
-      <c r="M63" s="68"/>
-      <c r="N63" s="68"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="36"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="36"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="62"/>
-      <c r="J64" s="62"/>
-      <c r="K64" s="62"/>
-      <c r="L64" s="62"/>
-      <c r="M64" s="62"/>
-      <c r="N64" s="62"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F65" s="90" t="s">
+      <c r="F65" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="G65" s="90"/>
-      <c r="H65" s="90"/>
-      <c r="I65" s="90"/>
-      <c r="J65" s="90"/>
-      <c r="K65" s="90"/>
-      <c r="L65" s="90"/>
-      <c r="M65" s="90"/>
-      <c r="N65" s="90"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F66" s="68"/>
-      <c r="G66" s="68"/>
-      <c r="H66" s="68"/>
-      <c r="I66" s="68"/>
-      <c r="J66" s="68"/>
-      <c r="K66" s="68"/>
-      <c r="L66" s="68"/>
-      <c r="M66" s="68"/>
-      <c r="N66" s="68"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="36"/>
+      <c r="J66" s="36"/>
+      <c r="K66" s="36"/>
+      <c r="L66" s="36"/>
+      <c r="M66" s="36"/>
+      <c r="N66" s="36"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="68" t="s">
+      <c r="A67" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="68"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="68"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="68"/>
-      <c r="H67" s="68"/>
-      <c r="I67" s="68"/>
-      <c r="J67" s="68"/>
-      <c r="K67" s="68"/>
-      <c r="L67" s="68"/>
-      <c r="M67" s="68"/>
-      <c r="N67" s="68"/>
-      <c r="O67" s="68"/>
-      <c r="P67" s="68"/>
-      <c r="Q67" s="68"/>
-      <c r="R67" s="68"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="36"/>
+      <c r="P67" s="36"/>
+      <c r="Q67" s="36"/>
+      <c r="R67" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="174">
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="P55:R55"/>
-    <mergeCell ref="P54:R54"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="P43:R43"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="F65:N65"/>
-    <mergeCell ref="F64:N64"/>
-    <mergeCell ref="E63:H63"/>
-    <mergeCell ref="B59:H59"/>
-    <mergeCell ref="P47:R47"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="P50:R50"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="O59:R59"/>
-    <mergeCell ref="O60:R60"/>
-    <mergeCell ref="A56:R56"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="P21:R22"/>
+    <mergeCell ref="F17:N20"/>
+    <mergeCell ref="O7:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="A21:E22"/>
+    <mergeCell ref="F21:H22"/>
+    <mergeCell ref="I21:O21"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="I66:K66"/>
+    <mergeCell ref="I57:K57"/>
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="I58:K58"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
     <mergeCell ref="P23:R23"/>
     <mergeCell ref="P24:R24"/>
     <mergeCell ref="P25:R25"/>
@@ -2606,116 +2787,46 @@
     <mergeCell ref="L43:N43"/>
     <mergeCell ref="L44:N44"/>
     <mergeCell ref="L45:N45"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="I66:K66"/>
-    <mergeCell ref="I57:K57"/>
-    <mergeCell ref="L37:N37"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="I58:K58"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="L29:N29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="A21:E22"/>
-    <mergeCell ref="F21:H22"/>
-    <mergeCell ref="I21:O21"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="P21:R22"/>
-    <mergeCell ref="F17:N20"/>
-    <mergeCell ref="O7:R10"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="F65:N65"/>
+    <mergeCell ref="F64:N64"/>
+    <mergeCell ref="E63:H63"/>
+    <mergeCell ref="B59:H59"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="P50:R50"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="O59:R59"/>
+    <mergeCell ref="O60:R60"/>
+    <mergeCell ref="A56:R56"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="P43:R43"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="P40:R40"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="P55:R55"/>
+    <mergeCell ref="P54:R54"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="14" scale="90" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>